<commit_message>
actualizare format + adaugare date
</commit_message>
<xml_diff>
--- a/Database/Cornestean/Europa.xlsx
+++ b/Database/Cornestean/Europa.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\horva\Desktop\Practica\Practica_covid19_UTCN\Database\Cornestean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AA9A1E-2B1F-4B4B-A3E9-6EFD600DD9D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BABE066C-1264-4543-A21D-1438993D7E6A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7010" yWindow="3710" windowWidth="26690" windowHeight="13640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,14 +591,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.7265625" customWidth="1"/>
-    <col min="2" max="17" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" customWidth="1"/>
+    <col min="3" max="17" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="19" max="178" width="10.26953125" bestFit="1" customWidth="1"/>
     <col min="179" max="179" width="14.1796875" customWidth="1"/>
@@ -609,11 +610,11 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -749,11 +750,11 @@
       </c>
     </row>
     <row r="2" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B2">
+      <c r="B2" s="9">
+        <v>43846</v>
+      </c>
+      <c r="C2">
         <v>1</v>
-      </c>
-      <c r="C2" s="9">
-        <v>43846</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="5"/>
@@ -801,11 +802,11 @@
       <c r="AV2" s="5"/>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B3">
+      <c r="B3" s="9">
+        <v>43847</v>
+      </c>
+      <c r="C3">
         <v>2</v>
-      </c>
-      <c r="C3" s="9">
-        <v>43847</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="5"/>
@@ -853,11 +854,11 @@
       <c r="AV3" s="5"/>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B4">
+      <c r="B4" s="9">
+        <v>43848</v>
+      </c>
+      <c r="C4">
         <v>3</v>
-      </c>
-      <c r="C4" s="9">
-        <v>43848</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="5"/>
@@ -905,11 +906,11 @@
       <c r="AV4" s="5"/>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B5">
+      <c r="B5" s="9">
+        <v>43849</v>
+      </c>
+      <c r="C5">
         <v>4</v>
-      </c>
-      <c r="C5" s="9">
-        <v>43849</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="5"/>
@@ -957,11 +958,11 @@
       <c r="AV5" s="5"/>
     </row>
     <row r="6" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B6">
+      <c r="B6" s="9">
+        <v>43850</v>
+      </c>
+      <c r="C6">
         <v>5</v>
-      </c>
-      <c r="C6" s="9">
-        <v>43850</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="5"/>
@@ -1009,11 +1010,11 @@
       <c r="AV6" s="5"/>
     </row>
     <row r="7" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B7">
+      <c r="B7" s="9">
+        <v>43851</v>
+      </c>
+      <c r="C7">
         <v>6</v>
-      </c>
-      <c r="C7" s="9">
-        <v>43851</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="5"/>
@@ -1061,11 +1062,11 @@
       <c r="AV7" s="5"/>
     </row>
     <row r="8" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B8">
+      <c r="B8" s="9">
+        <v>43852</v>
+      </c>
+      <c r="C8">
         <v>7</v>
-      </c>
-      <c r="C8" s="9">
-        <v>43852</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="5"/>
@@ -1113,11 +1114,11 @@
       <c r="AV8" s="5"/>
     </row>
     <row r="9" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B9">
+      <c r="B9" s="9">
+        <v>43853</v>
+      </c>
+      <c r="C9">
         <v>8</v>
-      </c>
-      <c r="C9" s="9">
-        <v>43853</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
@@ -1165,11 +1166,11 @@
       <c r="AV9" s="5"/>
     </row>
     <row r="10" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B10">
+      <c r="B10" s="9">
+        <v>43854</v>
+      </c>
+      <c r="C10">
         <v>9</v>
-      </c>
-      <c r="C10" s="9">
-        <v>43854</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
@@ -1219,11 +1220,11 @@
       <c r="AV10" s="5"/>
     </row>
     <row r="11" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B11">
+      <c r="B11" s="9">
+        <v>43855</v>
+      </c>
+      <c r="C11">
         <v>10</v>
-      </c>
-      <c r="C11" s="9">
-        <v>43855</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
@@ -1273,11 +1274,11 @@
       <c r="AV11" s="5"/>
     </row>
     <row r="12" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B12">
+      <c r="B12" s="9">
+        <v>43856</v>
+      </c>
+      <c r="C12">
         <v>11</v>
-      </c>
-      <c r="C12" s="9">
-        <v>43856</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
@@ -1325,11 +1326,11 @@
       <c r="AV12" s="5"/>
     </row>
     <row r="13" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B13">
+      <c r="B13" s="9">
+        <v>43857</v>
+      </c>
+      <c r="C13">
         <v>12</v>
-      </c>
-      <c r="C13" s="9">
-        <v>43857</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
@@ -1379,11 +1380,11 @@
       <c r="AV13" s="5"/>
     </row>
     <row r="14" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B14">
+      <c r="B14" s="9">
+        <v>43858</v>
+      </c>
+      <c r="C14">
         <v>13</v>
-      </c>
-      <c r="C14" s="9">
-        <v>43858</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="5"/>
@@ -1435,11 +1436,11 @@
       <c r="AV14" s="5"/>
     </row>
     <row r="15" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B15">
+      <c r="B15" s="9">
+        <v>43859</v>
+      </c>
+      <c r="C15">
         <v>14</v>
-      </c>
-      <c r="C15" s="9">
-        <v>43859</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="5"/>
@@ -1491,11 +1492,11 @@
       <c r="AV15" s="5"/>
     </row>
     <row r="16" spans="1:48" x14ac:dyDescent="0.35">
-      <c r="B16">
+      <c r="B16" s="9">
+        <v>43860</v>
+      </c>
+      <c r="C16">
         <v>15</v>
-      </c>
-      <c r="C16" s="9">
-        <v>43860</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="5"/>
@@ -1543,11 +1544,11 @@
       <c r="AV16" s="5"/>
     </row>
     <row r="17" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B17">
+      <c r="B17" s="9">
+        <v>43861</v>
+      </c>
+      <c r="C17">
         <v>16</v>
-      </c>
-      <c r="C17" s="9">
-        <v>43861</v>
       </c>
       <c r="E17" s="6">
         <v>2</v>
@@ -1605,11 +1606,11 @@
       <c r="AV17" s="5"/>
     </row>
     <row r="18" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B18">
+      <c r="B18" s="9">
+        <v>43862</v>
+      </c>
+      <c r="C18">
         <v>17</v>
-      </c>
-      <c r="C18" s="9">
-        <v>43862</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="5"/>
@@ -1663,11 +1664,11 @@
       <c r="AV18" s="5"/>
     </row>
     <row r="19" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B19">
+      <c r="B19" s="9">
+        <v>43863</v>
+      </c>
+      <c r="C19">
         <v>18</v>
-      </c>
-      <c r="C19" s="9">
-        <v>43863</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="5"/>
@@ -1717,11 +1718,11 @@
       <c r="AV19" s="5"/>
     </row>
     <row r="20" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B20">
+      <c r="B20" s="9">
+        <v>43864</v>
+      </c>
+      <c r="C20">
         <v>19</v>
-      </c>
-      <c r="C20" s="9">
-        <v>43864</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="5"/>
@@ -1771,11 +1772,11 @@
       <c r="AV20" s="5"/>
     </row>
     <row r="21" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B21">
+      <c r="B21" s="9">
+        <v>43865</v>
+      </c>
+      <c r="C21">
         <v>20</v>
-      </c>
-      <c r="C21" s="9">
-        <v>43865</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="5"/>
@@ -1825,11 +1826,11 @@
       <c r="AV21" s="5"/>
     </row>
     <row r="22" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B22">
+      <c r="B22" s="9">
+        <v>43866</v>
+      </c>
+      <c r="C22">
         <v>21</v>
-      </c>
-      <c r="C22" s="9">
-        <v>43866</v>
       </c>
       <c r="E22" s="6"/>
       <c r="F22" s="5"/>
@@ -1877,11 +1878,11 @@
       <c r="AV22" s="5"/>
     </row>
     <row r="23" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B23">
+      <c r="B23" s="9">
+        <v>43867</v>
+      </c>
+      <c r="C23">
         <v>22</v>
-      </c>
-      <c r="C23" s="9">
-        <v>43867</v>
       </c>
       <c r="E23" s="6"/>
       <c r="F23" s="5"/>
@@ -1929,11 +1930,11 @@
       <c r="AV23" s="5"/>
     </row>
     <row r="24" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B24">
+      <c r="B24" s="9">
+        <v>43868</v>
+      </c>
+      <c r="C24">
         <v>23</v>
-      </c>
-      <c r="C24" s="9">
-        <v>43868</v>
       </c>
       <c r="E24" s="6"/>
       <c r="F24" s="5">
@@ -1987,11 +1988,11 @@
       <c r="AV24" s="5"/>
     </row>
     <row r="25" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B25">
+      <c r="B25" s="9">
+        <v>43869</v>
+      </c>
+      <c r="C25">
         <v>24</v>
-      </c>
-      <c r="C25" s="9">
-        <v>43869</v>
       </c>
       <c r="E25" s="6"/>
       <c r="F25" s="5"/>
@@ -2041,11 +2042,11 @@
       <c r="AV25" s="5"/>
     </row>
     <row r="26" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B26">
+      <c r="B26" s="9">
+        <v>43870</v>
+      </c>
+      <c r="C26">
         <v>25</v>
-      </c>
-      <c r="C26" s="9">
-        <v>43870</v>
       </c>
       <c r="E26" s="6"/>
       <c r="F26" s="5"/>
@@ -2097,11 +2098,11 @@
       <c r="AV26" s="5"/>
     </row>
     <row r="27" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B27">
+      <c r="B27" s="9">
+        <v>43871</v>
+      </c>
+      <c r="C27">
         <v>26</v>
-      </c>
-      <c r="C27" s="9">
-        <v>43871</v>
       </c>
       <c r="E27" s="6"/>
       <c r="F27" s="5">
@@ -2151,11 +2152,11 @@
       <c r="AV27" s="5"/>
     </row>
     <row r="28" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B28">
+      <c r="B28" s="9">
+        <v>43872</v>
+      </c>
+      <c r="C28">
         <v>27</v>
-      </c>
-      <c r="C28" s="9">
-        <v>43872</v>
       </c>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
@@ -2205,11 +2206,11 @@
       <c r="AV28" s="5"/>
     </row>
     <row r="29" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B29">
+      <c r="B29" s="9">
+        <v>43873</v>
+      </c>
+      <c r="C29">
         <v>28</v>
-      </c>
-      <c r="C29" s="9">
-        <v>43873</v>
       </c>
       <c r="E29" s="6">
         <v>2</v>
@@ -2265,11 +2266,11 @@
       <c r="AV29" s="5"/>
     </row>
     <row r="30" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B30">
+      <c r="B30" s="9">
+        <v>43874</v>
+      </c>
+      <c r="C30">
         <v>29</v>
-      </c>
-      <c r="C30" s="9">
-        <v>43874</v>
       </c>
       <c r="E30" s="6"/>
       <c r="F30" s="5"/>
@@ -2319,11 +2320,11 @@
       <c r="AV30" s="5"/>
     </row>
     <row r="31" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B31">
+      <c r="B31" s="9">
+        <v>43875</v>
+      </c>
+      <c r="C31">
         <v>30</v>
-      </c>
-      <c r="C31" s="9">
-        <v>43875</v>
       </c>
       <c r="E31" s="6"/>
       <c r="F31" s="5"/>
@@ -2371,11 +2372,11 @@
       <c r="AV31" s="5"/>
     </row>
     <row r="32" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B32">
+      <c r="B32" s="9">
+        <v>43876</v>
+      </c>
+      <c r="C32">
         <v>31</v>
-      </c>
-      <c r="C32" s="9">
-        <v>43876</v>
       </c>
       <c r="E32" s="6"/>
       <c r="F32" s="5"/>
@@ -2427,11 +2428,11 @@
       <c r="AV32" s="5"/>
     </row>
     <row r="33" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B33">
+      <c r="B33" s="9">
+        <v>43877</v>
+      </c>
+      <c r="C33">
         <v>32</v>
-      </c>
-      <c r="C33" s="9">
-        <v>43877</v>
       </c>
       <c r="E33" s="6"/>
       <c r="F33" s="5">
@@ -2481,11 +2482,11 @@
       <c r="AV33" s="5"/>
     </row>
     <row r="34" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B34">
+      <c r="B34" s="9">
+        <v>43878</v>
+      </c>
+      <c r="C34">
         <v>33</v>
-      </c>
-      <c r="C34" s="9">
-        <v>43878</v>
       </c>
       <c r="E34" s="6"/>
       <c r="F34" s="5"/>
@@ -2535,11 +2536,11 @@
       <c r="AV34" s="5"/>
     </row>
     <row r="35" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B35">
+      <c r="B35" s="9">
+        <v>43879</v>
+      </c>
+      <c r="C35">
         <v>34</v>
-      </c>
-      <c r="C35" s="9">
-        <v>43879</v>
       </c>
       <c r="E35" s="6"/>
       <c r="F35" s="5"/>
@@ -2589,11 +2590,11 @@
       <c r="AV35" s="5"/>
     </row>
     <row r="36" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B36">
+      <c r="B36" s="9">
+        <v>43880</v>
+      </c>
+      <c r="C36">
         <v>35</v>
-      </c>
-      <c r="C36" s="9">
-        <v>43880</v>
       </c>
       <c r="E36" s="6"/>
       <c r="F36" s="5"/>
@@ -2641,11 +2642,11 @@
       <c r="AV36" s="5"/>
     </row>
     <row r="37" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B37">
+      <c r="B37" s="9">
+        <v>43881</v>
+      </c>
+      <c r="C37">
         <v>36</v>
-      </c>
-      <c r="C37" s="9">
-        <v>43881</v>
       </c>
       <c r="E37" s="6"/>
       <c r="F37" s="5"/>
@@ -2693,11 +2694,11 @@
       <c r="AV37" s="5"/>
     </row>
     <row r="38" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B38">
+      <c r="B38" s="9">
+        <v>43882</v>
+      </c>
+      <c r="C38">
         <v>37</v>
-      </c>
-      <c r="C38" s="9">
-        <v>43882</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="5"/>
@@ -2749,11 +2750,11 @@
       <c r="AV38" s="5"/>
     </row>
     <row r="39" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B39">
+      <c r="B39" s="9">
+        <v>43883</v>
+      </c>
+      <c r="C39">
         <v>38</v>
-      </c>
-      <c r="C39" s="9">
-        <v>43883</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="5"/>
@@ -2803,11 +2804,11 @@
       <c r="AV39" s="5"/>
     </row>
     <row r="40" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B40">
+      <c r="B40" s="9">
+        <v>43884</v>
+      </c>
+      <c r="C40">
         <v>39</v>
-      </c>
-      <c r="C40" s="9">
-        <v>43884</v>
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="5"/>
@@ -2857,11 +2858,11 @@
       <c r="AV40" s="5"/>
     </row>
     <row r="41" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B41">
+      <c r="B41" s="9">
+        <v>43885</v>
+      </c>
+      <c r="C41">
         <v>40</v>
-      </c>
-      <c r="C41" s="9">
-        <v>43885</v>
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="5">
@@ -2913,11 +2914,11 @@
       <c r="AV41" s="5"/>
     </row>
     <row r="42" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B42">
+      <c r="B42" s="9">
+        <v>43886</v>
+      </c>
+      <c r="C42">
         <v>41</v>
-      </c>
-      <c r="C42" s="9">
-        <v>43886</v>
       </c>
       <c r="E42" s="6"/>
       <c r="F42" s="5"/>
@@ -2979,11 +2980,11 @@
       <c r="AV42" s="5"/>
     </row>
     <row r="43" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B43">
+      <c r="B43" s="9">
+        <v>43887</v>
+      </c>
+      <c r="C43">
         <v>42</v>
-      </c>
-      <c r="C43" s="9">
-        <v>43887</v>
       </c>
       <c r="E43" s="6"/>
       <c r="F43" s="5"/>
@@ -3051,11 +3052,11 @@
       <c r="AV43" s="5"/>
     </row>
     <row r="44" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B44">
+      <c r="B44" s="9">
+        <v>43888</v>
+      </c>
+      <c r="C44">
         <v>43</v>
-      </c>
-      <c r="C44" s="9">
-        <v>43888</v>
       </c>
       <c r="E44" s="6"/>
       <c r="F44" s="5">
@@ -3129,11 +3130,11 @@
       <c r="AV44" s="5"/>
     </row>
     <row r="45" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B45">
+      <c r="B45" s="9">
+        <v>43889</v>
+      </c>
+      <c r="C45">
         <v>44</v>
-      </c>
-      <c r="C45" s="9">
-        <v>43889</v>
       </c>
       <c r="E45" s="6"/>
       <c r="F45" s="5">
@@ -3205,11 +3206,11 @@
       <c r="AV45" s="5"/>
     </row>
     <row r="46" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B46">
+      <c r="B46" s="9">
+        <v>43890</v>
+      </c>
+      <c r="C46">
         <v>45</v>
-      </c>
-      <c r="C46" s="9">
-        <v>43890</v>
       </c>
       <c r="E46" s="6"/>
       <c r="F46" s="5">
@@ -3289,11 +3290,11 @@
       <c r="AV46" s="5"/>
     </row>
     <row r="47" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B47">
+      <c r="B47" s="9">
+        <v>43891</v>
+      </c>
+      <c r="C47">
         <v>46</v>
-      </c>
-      <c r="C47" s="9">
-        <v>43891</v>
       </c>
       <c r="E47" s="6"/>
       <c r="F47" s="5">
@@ -3375,11 +3376,11 @@
       <c r="AV47" s="5"/>
     </row>
     <row r="48" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B48">
+      <c r="B48" s="9">
+        <v>43892</v>
+      </c>
+      <c r="C48">
         <v>47</v>
-      </c>
-      <c r="C48" s="9">
-        <v>43892</v>
       </c>
       <c r="E48" s="6">
         <v>3</v>
@@ -3461,11 +3462,11 @@
       <c r="AV48" s="5"/>
     </row>
     <row r="49" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B49">
+      <c r="B49" s="9">
+        <v>43893</v>
+      </c>
+      <c r="C49">
         <v>48</v>
-      </c>
-      <c r="C49" s="9">
-        <v>43893</v>
       </c>
       <c r="E49" s="6"/>
       <c r="F49" s="5">
@@ -3551,11 +3552,11 @@
       <c r="AV49" s="5"/>
     </row>
     <row r="50" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B50">
+      <c r="B50" s="9">
+        <v>43894</v>
+      </c>
+      <c r="C50">
         <v>49</v>
-      </c>
-      <c r="C50" s="9">
-        <v>43894</v>
       </c>
       <c r="E50" s="6"/>
       <c r="F50" s="5">
@@ -3649,11 +3650,11 @@
       <c r="AV50" s="5"/>
     </row>
     <row r="51" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B51">
+      <c r="B51" s="9">
+        <v>43895</v>
+      </c>
+      <c r="C51">
         <v>50</v>
-      </c>
-      <c r="C51" s="9">
-        <v>43895</v>
       </c>
       <c r="E51" s="6">
         <v>4</v>
@@ -3747,11 +3748,11 @@
       </c>
     </row>
     <row r="52" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B52">
+      <c r="B52" s="9">
+        <v>43896</v>
+      </c>
+      <c r="C52">
         <v>51</v>
-      </c>
-      <c r="C52" s="9">
-        <v>43896</v>
       </c>
       <c r="E52" s="6">
         <v>13</v>
@@ -3853,11 +3854,11 @@
       <c r="AV52" s="5"/>
     </row>
     <row r="53" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B53">
+      <c r="B53" s="9">
+        <v>43897</v>
+      </c>
+      <c r="C53">
         <v>52</v>
-      </c>
-      <c r="C53" s="9">
-        <v>43897</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="5">
@@ -3947,11 +3948,11 @@
       <c r="AV53" s="5"/>
     </row>
     <row r="54" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B54">
+      <c r="B54" s="9">
+        <v>43898</v>
+      </c>
+      <c r="C54">
         <v>53</v>
-      </c>
-      <c r="C54" s="9">
-        <v>43898</v>
       </c>
       <c r="E54" s="6">
         <v>17</v>
@@ -4055,11 +4056,11 @@
       <c r="AV54" s="5"/>
     </row>
     <row r="55" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B55">
+      <c r="B55" s="9">
+        <v>43899</v>
+      </c>
+      <c r="C55">
         <v>54</v>
-      </c>
-      <c r="C55" s="9">
-        <v>43899</v>
       </c>
       <c r="E55" s="6"/>
       <c r="F55" s="5">
@@ -4149,11 +4150,11 @@
       <c r="AV55" s="5"/>
     </row>
     <row r="56" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B56">
+      <c r="B56" s="9">
+        <v>43900</v>
+      </c>
+      <c r="C56">
         <v>55</v>
-      </c>
-      <c r="C56" s="9">
-        <v>43900</v>
       </c>
       <c r="E56" s="6">
         <v>10</v>
@@ -4271,11 +4272,11 @@
       <c r="AV56" s="5"/>
     </row>
     <row r="57" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B57">
+      <c r="B57" s="9">
+        <v>43901</v>
+      </c>
+      <c r="C57">
         <v>56</v>
-      </c>
-      <c r="C57" s="9">
-        <v>43901</v>
       </c>
       <c r="E57" s="6">
         <v>20</v>
@@ -4397,11 +4398,11 @@
       <c r="AV57" s="5"/>
     </row>
     <row r="58" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B58">
+      <c r="B58" s="9">
+        <v>43902</v>
+      </c>
+      <c r="C58">
         <v>57</v>
-      </c>
-      <c r="C58" s="9">
-        <v>43902</v>
       </c>
       <c r="E58" s="6">
         <v>28</v>
@@ -4493,11 +4494,11 @@
       <c r="AV58" s="5"/>
     </row>
     <row r="59" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B59">
+      <c r="B59" s="9">
+        <v>43903</v>
+      </c>
+      <c r="C59">
         <v>58</v>
-      </c>
-      <c r="C59" s="9">
-        <v>43903</v>
       </c>
       <c r="E59" s="6">
         <v>45</v>
@@ -4627,11 +4628,11 @@
       <c r="AV59" s="5"/>
     </row>
     <row r="60" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B60">
+      <c r="B60" s="9">
+        <v>43904</v>
+      </c>
+      <c r="C60">
         <v>59</v>
-      </c>
-      <c r="C60" s="9">
-        <v>43904</v>
       </c>
       <c r="E60" s="6">
         <v>59</v>
@@ -4757,11 +4758,11 @@
       </c>
     </row>
     <row r="61" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B61">
+      <c r="B61" s="9">
+        <v>43905</v>
+      </c>
+      <c r="C61">
         <v>60</v>
-      </c>
-      <c r="C61" s="9">
-        <v>43905</v>
       </c>
       <c r="E61" s="6">
         <v>63</v>
@@ -4881,11 +4882,11 @@
       <c r="AV61" s="5"/>
     </row>
     <row r="62" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B62">
+      <c r="B62" s="9">
+        <v>43906</v>
+      </c>
+      <c r="C62">
         <v>61</v>
-      </c>
-      <c r="C62" s="9">
-        <v>43906</v>
       </c>
       <c r="E62" s="6">
         <v>90</v>
@@ -5011,11 +5012,11 @@
       <c r="AV62" s="5"/>
     </row>
     <row r="63" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B63">
+      <c r="B63" s="9">
+        <v>43907</v>
+      </c>
+      <c r="C63">
         <v>62</v>
-      </c>
-      <c r="C63" s="9">
-        <v>43907</v>
       </c>
       <c r="E63" s="6">
         <v>114</v>
@@ -5145,11 +5146,11 @@
       </c>
     </row>
     <row r="64" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B64">
+      <c r="B64" s="9">
+        <v>43908</v>
+      </c>
+      <c r="C64">
         <v>63</v>
-      </c>
-      <c r="C64" s="9">
-        <v>43908</v>
       </c>
       <c r="E64" s="6">
         <v>147</v>
@@ -5273,11 +5274,11 @@
       </c>
     </row>
     <row r="65" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B65">
+      <c r="B65" s="9">
+        <v>43909</v>
+      </c>
+      <c r="C65">
         <v>64</v>
-      </c>
-      <c r="C65" s="9">
-        <v>43909</v>
       </c>
       <c r="E65" s="6">
         <v>199</v>
@@ -5405,11 +5406,11 @@
       <c r="AV65" s="5"/>
     </row>
     <row r="66" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B66">
+      <c r="B66" s="9">
+        <v>43910</v>
+      </c>
+      <c r="C66">
         <v>65</v>
-      </c>
-      <c r="C66" s="9">
-        <v>43910</v>
       </c>
       <c r="E66" s="6">
         <v>253</v>
@@ -5541,11 +5542,11 @@
       <c r="AV66" s="5"/>
     </row>
     <row r="67" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B67">
+      <c r="B67" s="9">
+        <v>43911</v>
+      </c>
+      <c r="C67">
         <v>66</v>
-      </c>
-      <c r="C67" s="9">
-        <v>43911</v>
       </c>
       <c r="E67" s="6">
         <v>306</v>
@@ -5677,11 +5678,11 @@
       </c>
     </row>
     <row r="68" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B68">
+      <c r="B68" s="9">
+        <v>43912</v>
+      </c>
+      <c r="C68">
         <v>67</v>
-      </c>
-      <c r="C68" s="9">
-        <v>43912</v>
       </c>
       <c r="E68" s="6">
         <v>367</v>
@@ -5813,11 +5814,11 @@
       <c r="AV68" s="5"/>
     </row>
     <row r="69" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B69">
+      <c r="B69" s="9">
+        <v>43913</v>
+      </c>
+      <c r="C69">
         <v>68</v>
-      </c>
-      <c r="C69" s="9">
-        <v>43913</v>
       </c>
       <c r="E69" s="6">
         <v>438</v>
@@ -5949,11 +5950,11 @@
       </c>
     </row>
     <row r="70" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B70">
+      <c r="B70" s="9">
+        <v>43914</v>
+      </c>
+      <c r="C70">
         <v>69</v>
-      </c>
-      <c r="C70" s="9">
-        <v>43914</v>
       </c>
       <c r="E70" s="6">
         <v>495</v>
@@ -6085,11 +6086,11 @@
       <c r="AV70" s="5"/>
     </row>
     <row r="71" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B71">
+      <c r="B71" s="9">
+        <v>43915</v>
+      </c>
+      <c r="C71">
         <v>70</v>
-      </c>
-      <c r="C71" s="9">
-        <v>43915</v>
       </c>
       <c r="E71" s="6">
         <v>658</v>
@@ -6223,11 +6224,11 @@
       <c r="AV71" s="5"/>
     </row>
     <row r="72" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B72">
+      <c r="B72" s="9">
+        <v>43916</v>
+      </c>
+      <c r="C72">
         <v>71</v>
-      </c>
-      <c r="C72" s="9">
-        <v>43916</v>
       </c>
       <c r="E72" s="6">
         <v>840</v>
@@ -6359,11 +6360,11 @@
       </c>
     </row>
     <row r="73" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B73">
+      <c r="B73" s="9">
+        <v>43917</v>
+      </c>
+      <c r="C73">
         <v>72</v>
-      </c>
-      <c r="C73" s="9">
-        <v>43917</v>
       </c>
       <c r="E73" s="6">
         <v>1036</v>
@@ -6497,11 +6498,11 @@
       <c r="AV73" s="5"/>
     </row>
     <row r="74" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B74">
+      <c r="B74" s="9">
+        <v>43918</v>
+      </c>
+      <c r="C74">
         <v>73</v>
-      </c>
-      <c r="C74" s="9">
-        <v>43918</v>
       </c>
       <c r="E74" s="6">
         <v>1264</v>
@@ -6631,11 +6632,11 @@
       <c r="AV74" s="5"/>
     </row>
     <row r="75" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B75">
+      <c r="B75" s="9">
+        <v>43919</v>
+      </c>
+      <c r="C75">
         <v>74</v>
-      </c>
-      <c r="C75" s="9">
-        <v>43919</v>
       </c>
       <c r="E75" s="6">
         <v>1534</v>
@@ -6765,11 +6766,11 @@
       <c r="AV75" s="5"/>
     </row>
     <row r="76" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B76">
+      <c r="B76" s="9">
+        <v>43920</v>
+      </c>
+      <c r="C76">
         <v>75</v>
-      </c>
-      <c r="C76" s="9">
-        <v>43920</v>
       </c>
       <c r="E76" s="6">
         <v>1836</v>
@@ -6905,11 +6906,11 @@
       </c>
     </row>
     <row r="77" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B77">
+      <c r="B77" s="9">
+        <v>43921</v>
+      </c>
+      <c r="C77">
         <v>76</v>
-      </c>
-      <c r="C77" s="9">
-        <v>43921</v>
       </c>
       <c r="E77" s="6">
         <v>2337</v>
@@ -7045,11 +7046,11 @@
       </c>
     </row>
     <row r="78" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B78">
+      <c r="B78" s="9">
+        <v>43922</v>
+      </c>
+      <c r="C78">
         <v>77</v>
-      </c>
-      <c r="C78" s="9">
-        <v>43922</v>
       </c>
       <c r="E78" s="6">
         <v>2777</v>
@@ -7181,11 +7182,11 @@
       <c r="AV78" s="5"/>
     </row>
     <row r="79" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B79">
+      <c r="B79" s="9">
+        <v>43923</v>
+      </c>
+      <c r="C79">
         <v>78</v>
-      </c>
-      <c r="C79" s="9">
-        <v>43923</v>
       </c>
       <c r="E79" s="6">
         <v>3548</v>
@@ -7321,11 +7322,11 @@
       </c>
     </row>
     <row r="80" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B80">
+      <c r="B80" s="9">
+        <v>43924</v>
+      </c>
+      <c r="C80">
         <v>79</v>
-      </c>
-      <c r="C80" s="9">
-        <v>43924</v>
       </c>
       <c r="E80" s="6">
         <v>4149</v>
@@ -7457,11 +7458,11 @@
       <c r="AV80" s="5"/>
     </row>
     <row r="81" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B81">
+      <c r="B81" s="9">
+        <v>43925</v>
+      </c>
+      <c r="C81">
         <v>80</v>
-      </c>
-      <c r="C81" s="9">
-        <v>43925</v>
       </c>
       <c r="E81" s="6">
         <v>4731</v>
@@ -7597,11 +7598,11 @@
       </c>
     </row>
     <row r="82" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B82">
+      <c r="B82" s="9">
+        <v>43926</v>
+      </c>
+      <c r="C82">
         <v>81</v>
-      </c>
-      <c r="C82" s="9">
-        <v>43926</v>
       </c>
       <c r="E82" s="6">
         <v>5389</v>
@@ -7735,11 +7736,11 @@
       <c r="AV82" s="5"/>
     </row>
     <row r="83" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B83">
+      <c r="B83" s="9">
+        <v>43927</v>
+      </c>
+      <c r="C83">
         <v>82</v>
-      </c>
-      <c r="C83" s="9">
-        <v>43927</v>
       </c>
       <c r="E83" s="6">
         <v>6343</v>
@@ -7873,11 +7874,11 @@
       </c>
     </row>
     <row r="84" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B84">
+      <c r="B84" s="9">
+        <v>43928</v>
+      </c>
+      <c r="C84">
         <v>83</v>
-      </c>
-      <c r="C84" s="9">
-        <v>43928</v>
       </c>
       <c r="E84" s="6">
         <v>7497</v>
@@ -8013,11 +8014,11 @@
       </c>
     </row>
     <row r="85" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B85">
+      <c r="B85" s="9">
+        <v>43929</v>
+      </c>
+      <c r="C85">
         <v>84</v>
-      </c>
-      <c r="C85" s="9">
-        <v>43929</v>
       </c>
       <c r="E85" s="6">
         <v>8672</v>
@@ -8149,11 +8150,11 @@
       <c r="AV85" s="5"/>
     </row>
     <row r="86" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B86">
+      <c r="B86" s="9">
+        <v>43930</v>
+      </c>
+      <c r="C86">
         <v>85</v>
-      </c>
-      <c r="C86" s="9">
-        <v>43930</v>
       </c>
       <c r="E86" s="6">
         <v>10131</v>
@@ -8287,11 +8288,11 @@
       <c r="AV86" s="5"/>
     </row>
     <row r="87" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B87">
+      <c r="B87" s="9">
+        <v>43931</v>
+      </c>
+      <c r="C87">
         <v>86</v>
-      </c>
-      <c r="C87" s="9">
-        <v>43931</v>
       </c>
       <c r="E87" s="6">
         <v>11917</v>
@@ -8427,11 +8428,11 @@
       </c>
     </row>
     <row r="88" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B88">
+      <c r="B88" s="9">
+        <v>43932</v>
+      </c>
+      <c r="C88">
         <v>87</v>
-      </c>
-      <c r="C88" s="9">
-        <v>43932</v>
       </c>
       <c r="E88" s="6">
         <v>13584</v>
@@ -8563,11 +8564,11 @@
       <c r="AV88" s="5"/>
     </row>
     <row r="89" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B89">
+      <c r="B89" s="9">
+        <v>43933</v>
+      </c>
+      <c r="C89">
         <v>88</v>
-      </c>
-      <c r="C89" s="9">
-        <v>43933</v>
       </c>
       <c r="E89" s="6">
         <v>15770</v>
@@ -8699,11 +8700,11 @@
       <c r="AV89" s="5"/>
     </row>
     <row r="90" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B90">
+      <c r="B90" s="9">
+        <v>43934</v>
+      </c>
+      <c r="C90">
         <v>89</v>
-      </c>
-      <c r="C90" s="9">
-        <v>43934</v>
       </c>
       <c r="E90" s="6">
         <v>18328</v>
@@ -8833,11 +8834,11 @@
       <c r="AV90" s="5"/>
     </row>
     <row r="91" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B91">
+      <c r="B91" s="9">
+        <v>43935</v>
+      </c>
+      <c r="C91">
         <v>90</v>
-      </c>
-      <c r="C91" s="9">
-        <v>43935</v>
       </c>
       <c r="E91" s="6">
         <v>21102</v>
@@ -8969,11 +8970,11 @@
       <c r="AV91" s="5"/>
     </row>
     <row r="92" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B92">
+      <c r="B92" s="9">
+        <v>43936</v>
+      </c>
+      <c r="C92">
         <v>91</v>
-      </c>
-      <c r="C92" s="9">
-        <v>43936</v>
       </c>
       <c r="E92" s="6">
         <v>24490</v>
@@ -9107,11 +9108,11 @@
       <c r="AV92" s="5"/>
     </row>
     <row r="93" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B93">
+      <c r="B93" s="9">
+        <v>43937</v>
+      </c>
+      <c r="C93">
         <v>92</v>
-      </c>
-      <c r="C93" s="9">
-        <v>43937</v>
       </c>
       <c r="E93" s="6">
         <v>27938</v>
@@ -9241,11 +9242,11 @@
       <c r="AV93" s="5"/>
     </row>
     <row r="94" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B94">
+      <c r="B94" s="9">
+        <v>43938</v>
+      </c>
+      <c r="C94">
         <v>93</v>
-      </c>
-      <c r="C94" s="9">
-        <v>43938</v>
       </c>
       <c r="E94" s="6">
         <v>32008</v>
@@ -9379,11 +9380,11 @@
       <c r="AV94" s="5"/>
     </row>
     <row r="95" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B95">
+      <c r="B95" s="9">
+        <v>43939</v>
+      </c>
+      <c r="C95">
         <v>94</v>
-      </c>
-      <c r="C95" s="9">
-        <v>43939</v>
       </c>
       <c r="E95" s="6">
         <v>36793</v>
@@ -9517,11 +9518,11 @@
       <c r="AV95" s="5"/>
     </row>
     <row r="96" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B96">
+      <c r="B96" s="9">
+        <v>43940</v>
+      </c>
+      <c r="C96">
         <v>95</v>
-      </c>
-      <c r="C96" s="9">
-        <v>43940</v>
       </c>
       <c r="E96" s="6">
         <v>42853</v>
@@ -9655,11 +9656,11 @@
       </c>
     </row>
     <row r="97" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B97">
+      <c r="B97" s="9">
+        <v>43941</v>
+      </c>
+      <c r="C97">
         <v>96</v>
-      </c>
-      <c r="C97" s="9">
-        <v>43941</v>
       </c>
       <c r="E97" s="6">
         <v>47121</v>
@@ -9793,11 +9794,11 @@
       <c r="AV97" s="5"/>
     </row>
     <row r="98" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B98">
+      <c r="B98" s="9">
+        <v>43942</v>
+      </c>
+      <c r="C98">
         <v>97</v>
-      </c>
-      <c r="C98" s="9">
-        <v>43942</v>
       </c>
       <c r="E98" s="6">
         <v>52763</v>
@@ -9931,11 +9932,11 @@
       <c r="AV98" s="5"/>
     </row>
     <row r="99" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B99">
+      <c r="B99" s="9">
+        <v>43943</v>
+      </c>
+      <c r="C99">
         <v>98</v>
-      </c>
-      <c r="C99" s="9">
-        <v>43943</v>
       </c>
       <c r="E99" s="6">
         <v>57999</v>
@@ -10067,11 +10068,11 @@
       <c r="AV99" s="5"/>
     </row>
     <row r="100" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B100">
+      <c r="B100" s="9">
+        <v>43944</v>
+      </c>
+      <c r="C100">
         <v>99</v>
-      </c>
-      <c r="C100" s="9">
-        <v>43944</v>
       </c>
       <c r="E100" s="6">
         <v>62773</v>
@@ -10205,11 +10206,11 @@
       <c r="AV100" s="5"/>
     </row>
     <row r="101" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B101">
+      <c r="B101" s="9">
+        <v>43945</v>
+      </c>
+      <c r="C101">
         <v>100</v>
-      </c>
-      <c r="C101" s="9">
-        <v>43945</v>
       </c>
       <c r="E101" s="6">
         <v>68622</v>
@@ -10343,11 +10344,11 @@
       <c r="AV101" s="5"/>
     </row>
     <row r="102" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B102">
+      <c r="B102" s="9">
+        <v>43946</v>
+      </c>
+      <c r="C102">
         <v>101</v>
-      </c>
-      <c r="C102" s="9">
-        <v>43946</v>
       </c>
       <c r="E102" s="6">
         <v>74588</v>
@@ -10477,11 +10478,11 @@
       <c r="AV102" s="5"/>
     </row>
     <row r="103" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B103">
+      <c r="B103" s="9">
+        <v>43947</v>
+      </c>
+      <c r="C103">
         <v>102</v>
-      </c>
-      <c r="C103" s="9">
-        <v>43947</v>
       </c>
       <c r="E103" s="6">
         <v>80949</v>
@@ -10611,11 +10612,11 @@
       <c r="AV103" s="5"/>
     </row>
     <row r="104" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B104">
+      <c r="B104" s="9">
+        <v>43948</v>
+      </c>
+      <c r="C104">
         <v>103</v>
-      </c>
-      <c r="C104" s="9">
-        <v>43948</v>
       </c>
       <c r="E104" s="6">
         <v>87147</v>
@@ -10747,11 +10748,11 @@
       <c r="AV104" s="5"/>
     </row>
     <row r="105" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B105">
+      <c r="B105" s="9">
+        <v>43949</v>
+      </c>
+      <c r="C105">
         <v>104</v>
-      </c>
-      <c r="C105" s="9">
-        <v>43949</v>
       </c>
       <c r="E105" s="6">
         <v>93558</v>
@@ -10885,11 +10886,11 @@
       <c r="AV105" s="5"/>
     </row>
     <row r="106" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B106">
+      <c r="B106" s="9">
+        <v>43950</v>
+      </c>
+      <c r="C106">
         <v>105</v>
-      </c>
-      <c r="C106" s="9">
-        <v>43950</v>
       </c>
       <c r="E106" s="6">
         <v>99399</v>
@@ -11023,11 +11024,11 @@
       <c r="AV106" s="5"/>
     </row>
     <row r="107" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B107">
+      <c r="B107" s="9">
+        <v>43951</v>
+      </c>
+      <c r="C107">
         <v>106</v>
-      </c>
-      <c r="C107" s="9">
-        <v>43951</v>
       </c>
       <c r="E107" s="6">
         <v>106498</v>
@@ -11161,11 +11162,11 @@
       <c r="AV107" s="5"/>
     </row>
     <row r="108" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B108">
+      <c r="B108" s="9">
+        <v>43952</v>
+      </c>
+      <c r="C108">
         <v>107</v>
-      </c>
-      <c r="C108" s="9">
-        <v>43952</v>
       </c>
       <c r="E108" s="6">
         <v>114431</v>
@@ -11295,11 +11296,11 @@
       <c r="AV108" s="5"/>
     </row>
     <row r="109" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B109">
+      <c r="B109" s="9">
+        <v>43953</v>
+      </c>
+      <c r="C109">
         <v>108</v>
-      </c>
-      <c r="C109" s="9">
-        <v>43953</v>
       </c>
       <c r="E109" s="6">
         <v>124054</v>
@@ -11433,11 +11434,11 @@
       <c r="AV109" s="5"/>
     </row>
     <row r="110" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B110">
+      <c r="B110" s="9">
+        <v>43954</v>
+      </c>
+      <c r="C110">
         <v>109</v>
-      </c>
-      <c r="C110" s="9">
-        <v>43954</v>
       </c>
       <c r="E110" s="6">
         <v>134687</v>
@@ -11569,11 +11570,11 @@
       <c r="AV110" s="5"/>
     </row>
     <row r="111" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B111">
+      <c r="B111" s="9">
+        <v>43955</v>
+      </c>
+      <c r="C111">
         <v>110</v>
-      </c>
-      <c r="C111" s="9">
-        <v>43955</v>
       </c>
       <c r="E111" s="6">
         <v>145268</v>
@@ -11703,11 +11704,11 @@
       <c r="AV111" s="5"/>
     </row>
     <row r="112" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B112">
+      <c r="B112" s="9">
+        <v>43956</v>
+      </c>
+      <c r="C112">
         <v>111</v>
-      </c>
-      <c r="C112" s="9">
-        <v>43956</v>
       </c>
       <c r="E112" s="6">
         <v>155370</v>
@@ -11841,11 +11842,11 @@
       <c r="AV112" s="5"/>
     </row>
     <row r="113" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B113">
+      <c r="B113" s="9">
+        <v>43957</v>
+      </c>
+      <c r="C113">
         <v>112</v>
-      </c>
-      <c r="C113" s="9">
-        <v>43957</v>
       </c>
       <c r="E113" s="6">
         <v>165929</v>
@@ -11979,11 +11980,11 @@
       <c r="AV113" s="5"/>
     </row>
     <row r="114" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B114">
+      <c r="B114" s="9">
+        <v>43958</v>
+      </c>
+      <c r="C114">
         <v>113</v>
-      </c>
-      <c r="C114" s="9">
-        <v>43958</v>
       </c>
       <c r="E114" s="6">
         <v>177160</v>
@@ -12115,11 +12116,11 @@
       <c r="AV114" s="5"/>
     </row>
     <row r="115" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B115">
+      <c r="B115" s="9">
+        <v>43959</v>
+      </c>
+      <c r="C115">
         <v>114</v>
-      </c>
-      <c r="C115" s="9">
-        <v>43959</v>
       </c>
       <c r="E115" s="6">
         <v>187859</v>
@@ -12251,11 +12252,11 @@
       <c r="AV115" s="5"/>
     </row>
     <row r="116" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B116">
+      <c r="B116" s="9">
+        <v>43960</v>
+      </c>
+      <c r="C116">
         <v>115</v>
-      </c>
-      <c r="C116" s="9">
-        <v>43960</v>
       </c>
       <c r="E116" s="6">
         <v>198676</v>
@@ -12389,11 +12390,11 @@
       <c r="AV116" s="5"/>
     </row>
     <row r="117" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B117">
+      <c r="B117" s="9">
+        <v>43961</v>
+      </c>
+      <c r="C117">
         <v>116</v>
-      </c>
-      <c r="C117" s="9">
-        <v>43961</v>
       </c>
       <c r="E117" s="6">
         <v>209688</v>
@@ -12521,11 +12522,11 @@
       <c r="AV117" s="5"/>
     </row>
     <row r="118" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B118">
+      <c r="B118" s="9">
+        <v>43962</v>
+      </c>
+      <c r="C118">
         <v>117</v>
-      </c>
-      <c r="C118" s="9">
-        <v>43962</v>
       </c>
       <c r="E118" s="6">
         <v>221344</v>
@@ -12655,11 +12656,11 @@
       <c r="AV118" s="5"/>
     </row>
     <row r="119" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B119">
+      <c r="B119" s="9">
+        <v>43963</v>
+      </c>
+      <c r="C119">
         <v>118</v>
-      </c>
-      <c r="C119" s="9">
-        <v>43963</v>
       </c>
       <c r="E119" s="6">
         <v>232243</v>
@@ -12791,11 +12792,11 @@
       <c r="AV119" s="5"/>
     </row>
     <row r="120" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B120">
+      <c r="B120" s="9">
+        <v>43964</v>
+      </c>
+      <c r="C120">
         <v>119</v>
-      </c>
-      <c r="C120" s="9">
-        <v>43964</v>
       </c>
       <c r="E120" s="6">
         <v>242271</v>
@@ -12929,11 +12930,11 @@
       <c r="AV120" s="5"/>
     </row>
     <row r="121" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B121">
+      <c r="B121" s="9">
+        <v>43965</v>
+      </c>
+      <c r="C121">
         <v>120</v>
-      </c>
-      <c r="C121" s="9">
-        <v>43965</v>
       </c>
       <c r="E121" s="6">
         <v>252245</v>
@@ -13063,11 +13064,11 @@
       <c r="AV121" s="5"/>
     </row>
     <row r="122" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B122">
+      <c r="B122" s="9">
+        <v>43966</v>
+      </c>
+      <c r="C122">
         <v>121</v>
-      </c>
-      <c r="C122" s="9">
-        <v>43966</v>
       </c>
       <c r="E122" s="6">
         <v>262843</v>
@@ -13199,11 +13200,11 @@
       <c r="AV122" s="5"/>
     </row>
     <row r="123" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B123">
+      <c r="B123" s="9">
+        <v>43967</v>
+      </c>
+      <c r="C123">
         <v>122</v>
-      </c>
-      <c r="C123" s="9">
-        <v>43967</v>
       </c>
       <c r="E123" s="6">
         <v>272043</v>
@@ -13333,11 +13334,11 @@
       <c r="AV123" s="5"/>
     </row>
     <row r="124" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B124">
+      <c r="B124" s="9">
+        <v>43968</v>
+      </c>
+      <c r="C124">
         <v>123</v>
-      </c>
-      <c r="C124" s="9">
-        <v>43968</v>
       </c>
       <c r="E124" s="6">
         <v>281752</v>
@@ -13463,11 +13464,11 @@
       <c r="AV124" s="5"/>
     </row>
     <row r="125" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B125">
+      <c r="B125" s="9">
+        <v>43969</v>
+      </c>
+      <c r="C125">
         <v>124</v>
-      </c>
-      <c r="C125" s="9">
-        <v>43969</v>
       </c>
       <c r="E125" s="6">
         <v>290678</v>
@@ -13597,11 +13598,11 @@
       <c r="AV125" s="5"/>
     </row>
     <row r="126" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B126">
+      <c r="B126" s="9">
+        <v>43970</v>
+      </c>
+      <c r="C126">
         <v>125</v>
-      </c>
-      <c r="C126" s="9">
-        <v>43970</v>
       </c>
       <c r="E126" s="6">
         <v>299941</v>
@@ -13733,11 +13734,11 @@
       <c r="AV126" s="5"/>
     </row>
     <row r="127" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B127">
+      <c r="B127" s="9">
+        <v>43971</v>
+      </c>
+      <c r="C127">
         <v>126</v>
-      </c>
-      <c r="C127" s="9">
-        <v>43971</v>
       </c>
       <c r="E127" s="6">
         <v>308705</v>
@@ -13869,11 +13870,11 @@
       <c r="AV127" s="5"/>
     </row>
     <row r="128" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B128">
+      <c r="B128" s="9">
+        <v>43972</v>
+      </c>
+      <c r="C128">
         <v>127</v>
-      </c>
-      <c r="C128" s="9">
-        <v>43972</v>
       </c>
       <c r="E128" s="6">
         <v>317554</v>
@@ -14003,11 +14004,11 @@
       <c r="AV128" s="5"/>
     </row>
     <row r="129" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B129">
+      <c r="B129" s="9">
+        <v>43973</v>
+      </c>
+      <c r="C129">
         <v>128</v>
-      </c>
-      <c r="C129" s="9">
-        <v>43973</v>
       </c>
       <c r="E129" s="6">
         <v>326448</v>
@@ -14135,11 +14136,11 @@
       <c r="AV129" s="5"/>
     </row>
     <row r="130" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B130">
+      <c r="B130" s="9">
+        <v>43974</v>
+      </c>
+      <c r="C130">
         <v>129</v>
-      </c>
-      <c r="C130" s="9">
-        <v>43974</v>
       </c>
       <c r="E130" s="6">
         <v>335882</v>
@@ -14269,11 +14270,11 @@
       <c r="AV130" s="5"/>
     </row>
     <row r="131" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B131">
+      <c r="B131" s="9">
+        <v>43975</v>
+      </c>
+      <c r="C131">
         <v>130</v>
-      </c>
-      <c r="C131" s="9">
-        <v>43975</v>
       </c>
       <c r="E131" s="6">
         <v>344481</v>
@@ -14399,11 +14400,11 @@
       <c r="AV131" s="5"/>
     </row>
     <row r="132" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B132">
+      <c r="B132" s="9">
+        <v>43976</v>
+      </c>
+      <c r="C132">
         <v>131</v>
-      </c>
-      <c r="C132" s="9">
-        <v>43976</v>
       </c>
       <c r="E132" s="6">
         <v>353427</v>
@@ -14531,11 +14532,11 @@
       <c r="AV132" s="5"/>
     </row>
     <row r="133" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B133">
+      <c r="B133" s="9">
+        <v>43977</v>
+      </c>
+      <c r="C133">
         <v>132</v>
-      </c>
-      <c r="C133" s="9">
-        <v>43977</v>
       </c>
       <c r="E133" s="6">
         <v>362342</v>
@@ -14663,11 +14664,11 @@
       <c r="AV133" s="5"/>
     </row>
     <row r="134" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B134">
+      <c r="B134" s="9">
+        <v>43978</v>
+      </c>
+      <c r="C134">
         <v>133</v>
-      </c>
-      <c r="C134" s="9">
-        <v>43978</v>
       </c>
       <c r="E134" s="6">
         <v>370680</v>
@@ -14791,11 +14792,11 @@
       <c r="AV134" s="5"/>
     </row>
     <row r="135" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B135">
+      <c r="B135" s="9">
+        <v>43979</v>
+      </c>
+      <c r="C135">
         <v>134</v>
-      </c>
-      <c r="C135" s="9">
-        <v>43979</v>
       </c>
       <c r="E135" s="6">
         <v>379051</v>
@@ -14923,11 +14924,11 @@
       <c r="AV135" s="5"/>
     </row>
     <row r="136" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B136">
+      <c r="B136" s="9">
+        <v>43980</v>
+      </c>
+      <c r="C136">
         <v>135</v>
-      </c>
-      <c r="C136" s="9">
-        <v>43980</v>
       </c>
       <c r="E136" s="6">
         <v>387623</v>
@@ -15057,11 +15058,11 @@
       <c r="AV136" s="5"/>
     </row>
     <row r="137" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B137">
+      <c r="B137" s="9">
+        <v>43981</v>
+      </c>
+      <c r="C137">
         <v>136</v>
-      </c>
-      <c r="C137" s="9">
-        <v>43981</v>
       </c>
       <c r="E137" s="6">
         <v>396575</v>
@@ -15191,11 +15192,11 @@
       <c r="AV137" s="5"/>
     </row>
     <row r="138" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B138">
+      <c r="B138" s="9">
+        <v>43982</v>
+      </c>
+      <c r="C138">
         <v>137</v>
-      </c>
-      <c r="C138" s="9">
-        <v>43982</v>
       </c>
       <c r="E138" s="6">
         <v>405843</v>
@@ -15319,11 +15320,11 @@
       <c r="AV138" s="5"/>
     </row>
     <row r="139" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B139">
+      <c r="B139" s="9">
+        <v>43983</v>
+      </c>
+      <c r="C139">
         <v>138</v>
-      </c>
-      <c r="C139" s="9">
-        <v>43983</v>
       </c>
       <c r="E139" s="6">
         <v>414328</v>
@@ -15449,11 +15450,11 @@
       <c r="AV139" s="5"/>
     </row>
     <row r="140" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B140">
+      <c r="B140" s="9">
+        <v>43984</v>
+      </c>
+      <c r="C140">
         <v>139</v>
-      </c>
-      <c r="C140" s="9">
-        <v>43984</v>
       </c>
       <c r="E140" s="6">
         <v>423186</v>
@@ -15581,11 +15582,11 @@
       <c r="AV140" s="5"/>
     </row>
     <row r="141" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B141">
+      <c r="B141" s="9">
+        <v>43985</v>
+      </c>
+      <c r="C141">
         <v>140</v>
-      </c>
-      <c r="C141" s="9">
-        <v>43985</v>
       </c>
       <c r="E141" s="6">
         <v>431715</v>
@@ -15711,11 +15712,11 @@
       <c r="AV141" s="5"/>
     </row>
     <row r="142" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B142">
+      <c r="B142" s="9">
+        <v>43986</v>
+      </c>
+      <c r="C142">
         <v>141</v>
-      </c>
-      <c r="C142" s="9">
-        <v>43986</v>
       </c>
       <c r="E142" s="6">
         <v>440538</v>
@@ -15843,11 +15844,11 @@
       <c r="AV142" s="5"/>
     </row>
     <row r="143" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B143">
+      <c r="B143" s="9">
+        <v>43987</v>
+      </c>
+      <c r="C143">
         <v>142</v>
-      </c>
-      <c r="C143" s="9">
-        <v>43987</v>
       </c>
       <c r="E143" s="6">
         <v>449256</v>
@@ -15977,11 +15978,11 @@
       <c r="AV143" s="5"/>
     </row>
     <row r="144" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B144">
+      <c r="B144" s="9">
+        <v>43988</v>
+      </c>
+      <c r="C144">
         <v>143</v>
-      </c>
-      <c r="C144" s="9">
-        <v>43988</v>
       </c>
       <c r="E144" s="6">
         <v>458102</v>
@@ -16103,11 +16104,11 @@
       <c r="AV144" s="5"/>
     </row>
     <row r="145" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B145">
+      <c r="B145" s="9">
+        <v>43989</v>
+      </c>
+      <c r="C145">
         <v>144</v>
-      </c>
-      <c r="C145" s="9">
-        <v>43989</v>
       </c>
       <c r="E145" s="6">
         <v>467073</v>
@@ -16233,11 +16234,11 @@
       <c r="AV145" s="5"/>
     </row>
     <row r="146" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B146">
+      <c r="B146" s="9">
+        <v>43990</v>
+      </c>
+      <c r="C146">
         <v>145</v>
-      </c>
-      <c r="C146" s="9">
-        <v>43990</v>
       </c>
       <c r="E146" s="6">
         <v>476043</v>
@@ -16363,11 +16364,11 @@
       <c r="AV146" s="5"/>
     </row>
     <row r="147" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B147">
+      <c r="B147" s="9">
+        <v>43991</v>
+      </c>
+      <c r="C147">
         <v>146</v>
-      </c>
-      <c r="C147" s="9">
-        <v>43991</v>
       </c>
       <c r="E147" s="6">
         <v>484630</v>
@@ -16495,11 +16496,11 @@
       <c r="AV147" s="5"/>
     </row>
     <row r="148" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B148">
+      <c r="B148" s="9">
+        <v>43992</v>
+      </c>
+      <c r="C148">
         <v>147</v>
-      </c>
-      <c r="C148" s="9">
-        <v>43992</v>
       </c>
       <c r="E148" s="6">
         <v>493023</v>
@@ -16627,11 +16628,11 @@
       <c r="AV148" s="5"/>
     </row>
     <row r="149" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B149">
+      <c r="B149" s="9">
+        <v>43993</v>
+      </c>
+      <c r="C149">
         <v>148</v>
-      </c>
-      <c r="C149" s="9">
-        <v>43993</v>
       </c>
       <c r="E149" s="6">
         <v>501800</v>
@@ -16755,11 +16756,11 @@
       <c r="AV149" s="5"/>
     </row>
     <row r="150" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B150">
+      <c r="B150" s="9">
+        <v>43994</v>
+      </c>
+      <c r="C150">
         <v>149</v>
-      </c>
-      <c r="C150" s="9">
-        <v>43994</v>
       </c>
       <c r="E150" s="6">
         <v>510761</v>
@@ -16887,11 +16888,11 @@
       <c r="AV150" s="5"/>
     </row>
     <row r="151" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B151">
+      <c r="B151" s="9">
+        <v>43995</v>
+      </c>
+      <c r="C151">
         <v>150</v>
-      </c>
-      <c r="C151" s="9">
-        <v>43995</v>
       </c>
       <c r="E151" s="6">
         <v>519458</v>
@@ -17013,11 +17014,11 @@
       <c r="AV151" s="5"/>
     </row>
     <row r="152" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B152">
+      <c r="B152" s="9">
+        <v>43996</v>
+      </c>
+      <c r="C152">
         <v>151</v>
-      </c>
-      <c r="C152" s="9">
-        <v>43996</v>
       </c>
       <c r="E152" s="6">
         <v>528267</v>
@@ -17139,11 +17140,11 @@
       <c r="AV152" s="5"/>
     </row>
     <row r="153" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B153">
+      <c r="B153" s="9">
+        <v>43997</v>
+      </c>
+      <c r="C153">
         <v>152</v>
-      </c>
-      <c r="C153" s="9">
-        <v>43997</v>
       </c>
       <c r="E153" s="6">
         <v>536484</v>
@@ -17271,11 +17272,11 @@
       <c r="AV153" s="5"/>
     </row>
     <row r="154" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B154">
+      <c r="B154" s="9">
+        <v>43998</v>
+      </c>
+      <c r="C154">
         <v>153</v>
-      </c>
-      <c r="C154" s="9">
-        <v>43998</v>
       </c>
       <c r="E154" s="6">
         <v>544725</v>
@@ -17407,11 +17408,11 @@
       <c r="AV154" s="5"/>
     </row>
     <row r="155" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B155">
+      <c r="B155" s="9">
+        <v>43999</v>
+      </c>
+      <c r="C155">
         <v>154</v>
-      </c>
-      <c r="C155" s="9">
-        <v>43999</v>
       </c>
       <c r="E155" s="6">
         <v>552549</v>
@@ -17541,11 +17542,11 @@
       <c r="AV155" s="5"/>
     </row>
     <row r="156" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B156">
+      <c r="B156" s="9">
+        <v>44000</v>
+      </c>
+      <c r="C156">
         <v>155</v>
-      </c>
-      <c r="C156" s="9">
-        <v>44000</v>
       </c>
       <c r="E156" s="6">
         <v>560321</v>
@@ -17677,11 +17678,11 @@
       <c r="AV156" s="5"/>
     </row>
     <row r="157" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B157">
+      <c r="B157" s="9">
+        <v>44001</v>
+      </c>
+      <c r="C157">
         <v>156</v>
-      </c>
-      <c r="C157" s="9">
-        <v>44001</v>
       </c>
       <c r="E157" s="6">
         <v>568292</v>
@@ -17809,11 +17810,11 @@
       <c r="AV157" s="5"/>
     </row>
     <row r="158" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B158">
+      <c r="B158" s="9">
+        <v>44002</v>
+      </c>
+      <c r="C158">
         <v>157</v>
-      </c>
-      <c r="C158" s="9">
-        <v>44002</v>
       </c>
       <c r="E158" s="6">
         <v>576162</v>
@@ -17937,11 +17938,11 @@
       <c r="AV158" s="5"/>
     </row>
     <row r="159" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B159">
+      <c r="B159" s="9">
+        <v>44003</v>
+      </c>
+      <c r="C159">
         <v>158</v>
-      </c>
-      <c r="C159" s="9">
-        <v>44003</v>
       </c>
       <c r="E159" s="6">
         <v>583879</v>
@@ -18063,11 +18064,11 @@
       <c r="AV159" s="5"/>
     </row>
     <row r="160" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B160">
+      <c r="B160" s="9">
+        <v>44004</v>
+      </c>
+      <c r="C160">
         <v>159</v>
-      </c>
-      <c r="C160" s="9">
-        <v>44004</v>
       </c>
       <c r="E160" s="6">
         <v>591465</v>
@@ -18197,11 +18198,11 @@
       </c>
     </row>
     <row r="161" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B161">
+      <c r="B161" s="9">
+        <v>44005</v>
+      </c>
+      <c r="C161">
         <v>160</v>
-      </c>
-      <c r="C161" s="9">
-        <v>44005</v>
       </c>
       <c r="E161" s="6">
         <v>598878</v>
@@ -18333,11 +18334,11 @@
       </c>
     </row>
     <row r="162" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B162">
+      <c r="B162" s="9">
+        <v>44006</v>
+      </c>
+      <c r="C162">
         <v>161</v>
-      </c>
-      <c r="C162" s="9">
-        <v>44006</v>
       </c>
       <c r="E162" s="6">
         <v>606043</v>
@@ -18467,11 +18468,11 @@
       </c>
     </row>
     <row r="163" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B163">
+      <c r="B163" s="9">
+        <v>44007</v>
+      </c>
+      <c r="C163">
         <v>162</v>
-      </c>
-      <c r="C163" s="9">
-        <v>44007</v>
       </c>
       <c r="E163" s="6">
         <v>613148</v>
@@ -18597,11 +18598,11 @@
       <c r="AV163" s="5"/>
     </row>
     <row r="164" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B164">
+      <c r="B164" s="9">
+        <v>44008</v>
+      </c>
+      <c r="C164">
         <v>163</v>
-      </c>
-      <c r="C164" s="9">
-        <v>44008</v>
       </c>
       <c r="E164" s="6">
         <v>619936</v>
@@ -18731,11 +18732,11 @@
       <c r="AV164" s="5"/>
     </row>
     <row r="165" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B165">
+      <c r="B165" s="9">
+        <v>44009</v>
+      </c>
+      <c r="C165">
         <v>164</v>
-      </c>
-      <c r="C165" s="9">
-        <v>44009</v>
       </c>
       <c r="E165" s="6">
         <v>626779</v>
@@ -18859,11 +18860,11 @@
       <c r="AV165" s="5"/>
     </row>
     <row r="166" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B166">
+      <c r="B166" s="9">
+        <v>44010</v>
+      </c>
+      <c r="C166">
         <v>165</v>
-      </c>
-      <c r="C166" s="9">
-        <v>44010</v>
       </c>
       <c r="E166" s="6">
         <v>633563</v>
@@ -18983,11 +18984,11 @@
       <c r="AV166" s="5"/>
     </row>
     <row r="167" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B167">
+      <c r="B167" s="9">
+        <v>44011</v>
+      </c>
+      <c r="C167">
         <v>166</v>
-      </c>
-      <c r="C167" s="9">
-        <v>44011</v>
       </c>
       <c r="E167" s="6">
         <v>640246</v>
@@ -19113,11 +19114,11 @@
       <c r="AV167" s="5"/>
     </row>
     <row r="168" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B168">
+      <c r="B168" s="9">
+        <v>44012</v>
+      </c>
+      <c r="C168">
         <v>167</v>
-      </c>
-      <c r="C168" s="9">
-        <v>44012</v>
       </c>
       <c r="E168" s="6">
         <v>646929</v>
@@ -19245,11 +19246,11 @@
       <c r="AV168" s="5"/>
     </row>
     <row r="169" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B169">
+      <c r="B169" s="9">
+        <v>44013</v>
+      </c>
+      <c r="C169">
         <v>168</v>
-      </c>
-      <c r="C169" s="9">
-        <v>44013</v>
       </c>
       <c r="E169" s="6">
         <v>653479</v>
@@ -19377,11 +19378,11 @@
       <c r="AV169" s="5"/>
     </row>
     <row r="170" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B170">
+      <c r="B170" s="9">
+        <v>44014</v>
+      </c>
+      <c r="C170">
         <v>169</v>
-      </c>
-      <c r="C170" s="9">
-        <v>44014</v>
       </c>
       <c r="E170" s="6">
         <v>660231</v>
@@ -19513,11 +19514,11 @@
       </c>
     </row>
     <row r="171" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B171">
+      <c r="B171" s="9">
+        <v>44015</v>
+      </c>
+      <c r="C171">
         <v>170</v>
-      </c>
-      <c r="C171" s="9">
-        <v>44015</v>
       </c>
       <c r="E171" s="6">
         <v>666941</v>
@@ -19645,11 +19646,11 @@
       <c r="AV171" s="5"/>
     </row>
     <row r="172" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B172">
+      <c r="B172" s="9">
+        <v>44016</v>
+      </c>
+      <c r="C172">
         <v>171</v>
-      </c>
-      <c r="C172" s="9">
-        <v>44016</v>
       </c>
       <c r="E172" s="6">
         <v>673564</v>
@@ -19769,11 +19770,11 @@
       <c r="AV172" s="5"/>
     </row>
     <row r="173" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B173">
+      <c r="B173" s="9">
+        <v>44017</v>
+      </c>
+      <c r="C173">
         <v>172</v>
-      </c>
-      <c r="C173" s="9">
-        <v>44017</v>
       </c>
       <c r="E173" s="6">
         <v>680283</v>
@@ -19895,11 +19896,11 @@
       <c r="AV173" s="5"/>
     </row>
     <row r="174" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B174">
+      <c r="B174" s="9">
+        <v>44018</v>
+      </c>
+      <c r="C174">
         <v>173</v>
-      </c>
-      <c r="C174" s="9">
-        <v>44018</v>
       </c>
       <c r="E174" s="6">
         <v>686852</v>
@@ -20027,11 +20028,11 @@
       </c>
     </row>
     <row r="175" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B175">
+      <c r="B175" s="9">
+        <v>44019</v>
+      </c>
+      <c r="C175">
         <v>174</v>
-      </c>
-      <c r="C175" s="9">
-        <v>44019</v>
       </c>
       <c r="E175" s="6">
         <v>693215</v>
@@ -20159,11 +20160,11 @@
       <c r="AV175" s="5"/>
     </row>
     <row r="176" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B176">
+      <c r="B176" s="9">
+        <v>44020</v>
+      </c>
+      <c r="C176">
         <v>175</v>
-      </c>
-      <c r="C176" s="9">
-        <v>44020</v>
       </c>
       <c r="E176" s="6">
         <v>699749</v>
@@ -20293,11 +20294,11 @@
       <c r="AV176" s="5"/>
     </row>
     <row r="177" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B177">
+      <c r="B177" s="9">
+        <v>44021</v>
+      </c>
+      <c r="C177">
         <v>176</v>
-      </c>
-      <c r="C177" s="9">
-        <v>44021</v>
       </c>
       <c r="E177" s="6">
         <v>706240</v>
@@ -20429,11 +20430,11 @@
       <c r="AV177" s="5"/>
     </row>
     <row r="178" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B178">
+      <c r="B178" s="9">
+        <v>44022</v>
+      </c>
+      <c r="C178">
         <v>177</v>
-      </c>
-      <c r="C178" s="9">
-        <v>44022</v>
       </c>
       <c r="E178" s="6">
         <v>712863</v>
@@ -20561,11 +20562,11 @@
       <c r="AV178" s="5"/>
     </row>
     <row r="179" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B179">
+      <c r="B179" s="9">
+        <v>44023</v>
+      </c>
+      <c r="C179">
         <v>178</v>
-      </c>
-      <c r="C179" s="9">
-        <v>44023</v>
       </c>
       <c r="E179" s="6">
         <v>719449</v>
@@ -20687,11 +20688,11 @@
       <c r="AV179" s="5"/>
     </row>
     <row r="180" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B180">
+      <c r="B180" s="9">
+        <v>44024</v>
+      </c>
+      <c r="C180">
         <v>179</v>
-      </c>
-      <c r="C180" s="9">
-        <v>44024</v>
       </c>
       <c r="E180" s="6">
         <v>726036</v>
@@ -20811,11 +20812,11 @@
       <c r="AV180" s="5"/>
     </row>
     <row r="181" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B181">
+      <c r="B181" s="9">
+        <v>44025</v>
+      </c>
+      <c r="C181">
         <v>180</v>
-      </c>
-      <c r="C181" s="9">
-        <v>44025</v>
       </c>
       <c r="E181" s="6">
         <v>732547</v>
@@ -20939,11 +20940,11 @@
       <c r="AV181" s="5"/>
     </row>
     <row r="182" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B182">
+      <c r="B182" s="9">
+        <v>44026</v>
+      </c>
+      <c r="C182">
         <v>181</v>
-      </c>
-      <c r="C182" s="9">
-        <v>44026</v>
       </c>
       <c r="E182" s="6">
         <v>738787</v>
@@ -21067,11 +21068,11 @@
       <c r="AV182" s="5"/>
     </row>
     <row r="183" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B183">
+      <c r="B183" s="9">
+        <v>44027</v>
+      </c>
+      <c r="C183">
         <v>182</v>
-      </c>
-      <c r="C183" s="9">
-        <v>44027</v>
       </c>
       <c r="E183" s="6">
         <v>745197</v>
@@ -21199,11 +21200,11 @@
       <c r="AV183" s="5"/>
     </row>
     <row r="184" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B184">
+      <c r="B184" s="9">
+        <v>44028</v>
+      </c>
+      <c r="C184">
         <v>183</v>
-      </c>
-      <c r="C184" s="9">
-        <v>44028</v>
       </c>
       <c r="E184" s="6">
         <v>751612</v>
@@ -21331,11 +21332,11 @@
       <c r="AV184" s="5"/>
     </row>
     <row r="185" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B185">
+      <c r="B185" s="9">
+        <v>44029</v>
+      </c>
+      <c r="C185">
         <v>184</v>
-      </c>
-      <c r="C185" s="9">
-        <v>44029</v>
       </c>
       <c r="E185" s="6">
         <v>758001</v>
@@ -21467,11 +21468,11 @@
       </c>
     </row>
     <row r="186" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B186">
+      <c r="B186" s="9">
+        <v>44030</v>
+      </c>
+      <c r="C186">
         <v>185</v>
-      </c>
-      <c r="C186" s="9">
-        <v>44030</v>
       </c>
       <c r="E186" s="6">
         <v>764215</v>
@@ -21595,11 +21596,11 @@
       </c>
     </row>
     <row r="187" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B187">
+      <c r="B187" s="9">
+        <v>44031</v>
+      </c>
+      <c r="C187">
         <v>186</v>
-      </c>
-      <c r="C187" s="9">
-        <v>44031</v>
       </c>
       <c r="E187" s="6">
         <v>770311</v>
@@ -21715,11 +21716,11 @@
       <c r="AV187" s="5"/>
     </row>
     <row r="188" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B188">
+      <c r="B188" s="9">
+        <v>44032</v>
+      </c>
+      <c r="C188">
         <v>187</v>
-      </c>
-      <c r="C188" s="9">
-        <v>44032</v>
       </c>
       <c r="E188" s="6">
         <v>776212</v>
@@ -21843,11 +21844,11 @@
       <c r="AV188" s="5"/>
     </row>
     <row r="189" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B189">
+      <c r="B189" s="9">
+        <v>44033</v>
+      </c>
+      <c r="C189">
         <v>188</v>
-      </c>
-      <c r="C189" s="9">
-        <v>44033</v>
       </c>
       <c r="E189" s="6">
         <v>782040</v>
@@ -21975,11 +21976,11 @@
       <c r="AV189" s="5"/>
     </row>
     <row r="190" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B190">
+      <c r="B190" s="9">
+        <v>44034</v>
+      </c>
+      <c r="C190">
         <v>189</v>
-      </c>
-      <c r="C190" s="9">
-        <v>44034</v>
       </c>
       <c r="E190" s="6">
         <v>787890</v>
@@ -22111,11 +22112,11 @@
       </c>
     </row>
     <row r="191" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B191">
+      <c r="B191" s="9">
+        <v>44035</v>
+      </c>
+      <c r="C191">
         <v>190</v>
-      </c>
-      <c r="C191" s="9">
-        <v>44035</v>
       </c>
       <c r="E191" s="6">
         <v>793720</v>
@@ -22245,11 +22246,11 @@
       <c r="AV191" s="5"/>
     </row>
     <row r="192" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B192">
+      <c r="B192" s="9">
+        <v>44036</v>
+      </c>
+      <c r="C192">
         <v>191</v>
-      </c>
-      <c r="C192" s="9">
-        <v>44036</v>
       </c>
       <c r="E192" s="6">
         <v>799499</v>
@@ -22383,11 +22384,11 @@
       <c r="AV192" s="5"/>
     </row>
     <row r="193" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B193">
+      <c r="B193" s="9">
+        <v>44037</v>
+      </c>
+      <c r="C193">
         <v>192</v>
-      </c>
-      <c r="C193" s="9">
-        <v>44037</v>
       </c>
       <c r="E193" s="6">
         <v>805332</v>
@@ -22503,11 +22504,11 @@
       <c r="AV193" s="5"/>
     </row>
     <row r="194" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B194">
+      <c r="B194" s="9">
+        <v>44038</v>
+      </c>
+      <c r="C194">
         <v>193</v>
-      </c>
-      <c r="C194" s="9">
-        <v>44038</v>
       </c>
       <c r="E194" s="6">
         <v>811073</v>
@@ -22625,11 +22626,11 @@
       <c r="AV194" s="5"/>
     </row>
     <row r="195" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B195">
+      <c r="B195" s="9">
+        <v>44039</v>
+      </c>
+      <c r="C195">
         <v>194</v>
-      </c>
-      <c r="C195" s="9">
-        <v>44039</v>
       </c>
       <c r="E195" s="6">
         <v>816680</v>
@@ -22757,11 +22758,11 @@
       <c r="AV195" s="5"/>
     </row>
     <row r="196" spans="2:48" x14ac:dyDescent="0.35">
-      <c r="B196">
+      <c r="B196" s="9">
+        <v>44040</v>
+      </c>
+      <c r="C196">
         <v>195</v>
-      </c>
-      <c r="C196" s="9">
-        <v>44040</v>
       </c>
       <c r="E196" s="10">
         <v>822060</v>

</xml_diff>